<commit_message>
Contenido hasta semana 4
</commit_message>
<xml_diff>
--- a/Estudiantes.xlsx
+++ b/Estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSE\Desktop\Trabajo\Herramientas\HCAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F13E42-51CF-470A-A207-9DE4B2C8636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744E0218-19BE-420D-99FB-5C03D74B37B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1335" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="136">
   <si>
     <t>Nombre</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Estudiante</t>
   </si>
   <si>
+    <t>Camilo-AndradePerez</t>
+  </si>
+  <si>
     <t>Aramendiz Guzman, Ana Maria</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
     <t>l.caballeroo</t>
   </si>
   <si>
+    <t>LauraCaballero14</t>
+  </si>
+  <si>
     <t>Calderon Gasca, Andres Felipe</t>
   </si>
   <si>
@@ -150,6 +156,9 @@
     <t>m.flechas</t>
   </si>
   <si>
+    <t>maflecha</t>
+  </si>
+  <si>
     <t>Franco Nino, Kevin Yesid</t>
   </si>
   <si>
@@ -165,6 +174,9 @@
     <t>j.franco10</t>
   </si>
   <si>
+    <t>javierfranco27</t>
+  </si>
+  <si>
     <t>Gallego Leon, Juan Sebastian</t>
   </si>
   <si>
@@ -282,6 +294,9 @@
     <t>a.penah</t>
   </si>
   <si>
+    <t>Arpenahi</t>
+  </si>
+  <si>
     <t>Penaranda Saddy, Camilo Andres</t>
   </si>
   <si>
@@ -315,12 +330,18 @@
     <t>li.pinilla685</t>
   </si>
   <si>
+    <t>lipinilla685</t>
+  </si>
+  <si>
     <t>Rangel, Holguer Yahir</t>
   </si>
   <si>
     <t>h.rangel</t>
   </si>
   <si>
+    <t>HolguerRangel</t>
+  </si>
+  <si>
     <t>Restrepo Salazar, Nicolas </t>
   </si>
   <si>
@@ -336,6 +357,9 @@
     <t>cm.rincon170</t>
   </si>
   <si>
+    <t>mrincon19</t>
+  </si>
+  <si>
     <t>Rodriguez Tique, Daniel Hernando</t>
   </si>
   <si>
@@ -351,6 +375,9 @@
     <t>sa.rojass</t>
   </si>
   <si>
+    <t>stephanierojas1234</t>
+  </si>
+  <si>
     <t>Sanabria Morales, Diana Carolina</t>
   </si>
   <si>
@@ -364,6 +391,9 @@
   </si>
   <si>
     <t>l.sanchezd</t>
+  </si>
+  <si>
+    <t>LauraSanchez9585</t>
   </si>
   <si>
     <t>Torres Torres, Camilo Andres</t>
@@ -412,7 +442,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +478,11 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -512,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -528,9 +563,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -858,7 +894,7 @@
   <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -908,13 +944,16 @@
       <c r="E2" s="7">
         <v>1</v>
       </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6">
         <v>202124465</v>
@@ -926,15 +965,15 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6">
         <v>201511452</v>
@@ -946,15 +985,15 @@
         <v>3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6">
         <v>202125018</v>
@@ -965,16 +1004,16 @@
       <c r="E5" s="7">
         <v>4</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
+      <c r="F5" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6">
         <v>201411968</v>
@@ -986,15 +1025,15 @@
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6">
         <v>202124253</v>
@@ -1005,13 +1044,16 @@
       <c r="E7" s="7">
         <v>6</v>
       </c>
+      <c r="F7" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6">
         <v>202125023</v>
@@ -1023,15 +1065,15 @@
         <v>7</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6">
         <v>201211959</v>
@@ -1043,15 +1085,15 @@
         <v>8</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6">
         <v>202120851</v>
@@ -1063,15 +1105,15 @@
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="6">
         <v>202124223</v>
@@ -1083,15 +1125,15 @@
         <v>10</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6">
         <v>201111892</v>
@@ -1103,15 +1145,15 @@
         <v>11</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="6">
         <v>202120855</v>
@@ -1122,13 +1164,16 @@
       <c r="E13" s="7">
         <v>12</v>
       </c>
+      <c r="F13" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6">
         <v>202027566</v>
@@ -1140,15 +1185,15 @@
         <v>13</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C15" s="6">
         <v>201320220</v>
@@ -1159,13 +1204,16 @@
       <c r="E15" s="7">
         <v>14</v>
       </c>
+      <c r="F15" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="14.25" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6">
         <v>201218621</v>
@@ -1177,15 +1225,15 @@
         <v>15</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6">
         <v>201413450</v>
@@ -1197,15 +1245,15 @@
         <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6">
         <v>201023060</v>
@@ -1217,15 +1265,15 @@
         <v>17</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6">
         <v>202121034</v>
@@ -1237,15 +1285,15 @@
         <v>18</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C20" s="6">
         <v>202125039</v>
@@ -1259,10 +1307,10 @@
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6">
         <v>201023106</v>
@@ -1274,15 +1322,15 @@
         <v>20</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C22" s="6">
         <v>202120647</v>
@@ -1294,15 +1342,15 @@
         <v>21</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C23" s="6">
         <v>202125046</v>
@@ -1314,15 +1362,15 @@
         <v>22</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C24" s="6">
         <v>201118377</v>
@@ -1333,16 +1381,16 @@
       <c r="E24" s="7">
         <v>23</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>70</v>
+      <c r="F24" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C25" s="6">
         <v>201015520</v>
@@ -1356,10 +1404,10 @@
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C26" s="6">
         <v>202125057</v>
@@ -1371,15 +1419,15 @@
         <v>25</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C27" s="6">
         <v>202124531</v>
@@ -1391,15 +1439,15 @@
         <v>26</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C28" s="6">
         <v>202124968</v>
@@ -1410,16 +1458,16 @@
       <c r="E28" s="7">
         <v>27</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>81</v>
+      <c r="F28" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C29" s="6">
         <v>201629144</v>
@@ -1430,13 +1478,16 @@
       <c r="E29" s="7">
         <v>28</v>
       </c>
+      <c r="F29" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6">
         <v>202120871</v>
@@ -1448,15 +1499,15 @@
         <v>29</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C31" s="6">
         <v>202124460</v>
@@ -1468,15 +1519,15 @@
         <v>30</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C32" s="6">
         <v>202028074</v>
@@ -1487,16 +1538,16 @@
       <c r="E32" s="7">
         <v>31</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>92</v>
+      <c r="F32" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C33" s="6">
         <v>201217337</v>
@@ -1507,13 +1558,16 @@
       <c r="E33" s="7">
         <v>32</v>
       </c>
+      <c r="F33" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A34" s="11" t="s">
-        <v>95</v>
+      <c r="A34" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C34" s="6">
         <v>202110106</v>
@@ -1524,13 +1578,16 @@
       <c r="E34" s="7">
         <v>33</v>
       </c>
+      <c r="F34" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C35" s="6">
         <v>201216368</v>
@@ -1542,15 +1599,15 @@
         <v>34</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C36" s="6">
         <v>200722149</v>
@@ -1561,13 +1618,16 @@
       <c r="E36" s="7">
         <v>35</v>
       </c>
+      <c r="F36" s="7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C37" s="6">
         <v>202124972</v>
@@ -1579,15 +1639,15 @@
         <v>36</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C38" s="6">
         <v>202125073</v>
@@ -1598,13 +1658,16 @@
       <c r="E38" s="7">
         <v>37</v>
       </c>
+      <c r="F38" s="7" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C39" s="6">
         <v>202124973</v>
@@ -1616,15 +1679,15 @@
         <v>38</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C40" s="6">
         <v>201215030</v>
@@ -1635,13 +1698,16 @@
       <c r="E40" s="7">
         <v>39</v>
       </c>
+      <c r="F40" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C41" s="6">
         <v>201215238</v>
@@ -1653,15 +1719,15 @@
         <v>40</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C42" s="6">
         <v>202120697</v>
@@ -1673,15 +1739,15 @@
         <v>41</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.25" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C43" s="6">
         <v>202121068</v>
@@ -1693,15 +1759,15 @@
         <v>42</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C44" s="6">
         <v>202116276</v>
@@ -1713,15 +1779,15 @@
         <v>43</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C45" s="6">
         <v>202028138</v>

</xml_diff>